<commit_message>
Bulk upload voters is now working!!!
</commit_message>
<xml_diff>
--- a/public/assets/excel/voters_sample.xlsx
+++ b/public/assets/excel/voters_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brice\Documents\GitHub\eboto-mo\public\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82344F9D-1F3F-4883-8A59-8A7ED97E345A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6E490A-8F82-4D1A-9550-9D83F7AF4882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36495" yWindow="660" windowWidth="21345" windowHeight="12915" xr2:uid="{D3986BDA-9B48-47DA-B0E3-B07B8A502D56}"/>
+    <workbookView xWindow="35805" yWindow="1125" windowWidth="21345" windowHeight="12915" xr2:uid="{D3986BDA-9B48-47DA-B0E3-B07B8A502D56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Full name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>juan.delacruz@cvsu.edu.ph</t>
   </si>
   <si>
@@ -51,6 +45,12 @@
   </si>
   <si>
     <t>pedro.penduko@cvsu.edu.ph</t>
+  </si>
+  <si>
+    <t>full_name</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -416,7 +416,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -427,26 +427,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>